<commit_message>
Ajusted mvp-requisitos, cadastre-se form and fixed avaliacao.html button
</commit_message>
<xml_diff>
--- a/ATIVIDADES/mvp-requisitos.xlsx
+++ b/ATIVIDADES/mvp-requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lucas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lucas\Desktop\PROJETO MVP FRONT\AgendaFacilNaf\ATIVIDADES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Tipo do Requisito</t>
   </si>
@@ -59,18 +59,12 @@
     <t>O sistema deve ser responsivo para smartphones;</t>
   </si>
   <si>
-    <t>O sistema deve exibir a página de usuário com as seguintes opções de login: Estudante, Porfessor e Administrador;</t>
-  </si>
-  <si>
     <t>O sistema deve ser ituitivo e fácil de usar, com cores confortáveis e informações objetivas;</t>
   </si>
   <si>
     <t>O sistema não deve permitir que o usuário se conecte simultaneamente em aparelhos distintos  com o mesmo login;</t>
   </si>
   <si>
-    <t>O sistema deve permitir a criação de relatórios em pdf com todos os agendamentos personalizados;</t>
-  </si>
-  <si>
     <t>O sistema deve ficar disponível, no mínimo, 95% do tempo anual, eventuais manutenções deverão ocorrer de preferência no período noturno de menor atividade;</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>O sistema deve permitir que um usuário logado avalie o atendimento;</t>
   </si>
   <si>
-    <t>O sistema deve permitir que qualquer pessoa posso se cadastrar;</t>
-  </si>
-  <si>
     <t>O  sistema deve ser desenvolvido com as seguintes tecnologias Front-End: Html, Css e JavaScript;</t>
   </si>
   <si>
@@ -99,6 +90,12 @@
   </si>
   <si>
     <t>O sistema deve permitir que Professores e Estudantes, com login efetuado, consigam acessar uma tabela com os dados dos agendamentos atribuídos à eles pelo administrador;</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir a página de usuário com as seguintes opções de login: Login do cliente, Estudante, Porfessor e Administrador;</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que qualquer pessoa possa se cadastrar;</t>
   </si>
 </sst>
 </file>
@@ -479,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -508,7 +505,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -553,7 +550,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -564,7 +561,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -575,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -586,7 +583,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -597,7 +594,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -612,52 +609,51 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="72.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -668,31 +664,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>